<commit_message>
Preparado para CESA pt1
</commit_message>
<xml_diff>
--- a/data/partidos/partidos_CESA23IM.xlsx
+++ b/data/partidos/partidos_CESA23IM.xlsx
@@ -4332,7 +4332,7 @@
       </c>
       <c r="JO4" t="inlineStr">
         <is>
-          <t>AIANTZE AYESA JUSTICIA</t>
+          <t>BITTOR ARANAZ HERNANDEZ</t>
         </is>
       </c>
       <c r="JP4" t="inlineStr"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="JS4" t="inlineStr">
         <is>
-          <t>BITTOR ARANAZ HERNANDEZ</t>
+          <t>AIANTZE AYESA JUSTICIA</t>
         </is>
       </c>
       <c r="JT4" t="inlineStr"/>
@@ -10037,37 +10037,37 @@
       </c>
       <c r="JM11" t="inlineStr">
         <is>
+          <t>SANTIAGO DE LA VARGA NICOLAS</t>
+        </is>
+      </c>
+      <c r="JN11" t="inlineStr">
+        <is>
+          <t>OFICIAL</t>
+        </is>
+      </c>
+      <c r="JO11" t="inlineStr">
+        <is>
+          <t>FRANCISCO JAVIER LOPEZ GUERRERO</t>
+        </is>
+      </c>
+      <c r="JP11" t="inlineStr">
+        <is>
+          <t>OFICIAL</t>
+        </is>
+      </c>
+      <c r="JQ11" t="inlineStr">
+        <is>
           <t>ALEJANDRO OLIVA LASECA</t>
         </is>
       </c>
-      <c r="JN11" t="inlineStr">
+      <c r="JR11" t="inlineStr">
         <is>
           <t>OFICIAL</t>
         </is>
       </c>
-      <c r="JO11" t="inlineStr">
+      <c r="JS11" t="inlineStr">
         <is>
           <t>MARIA DEL CARMEN BUENO NOGALES</t>
-        </is>
-      </c>
-      <c r="JP11" t="inlineStr">
-        <is>
-          <t>OFICIAL</t>
-        </is>
-      </c>
-      <c r="JQ11" t="inlineStr">
-        <is>
-          <t>SANTIAGO DE LA VARGA NICOLAS</t>
-        </is>
-      </c>
-      <c r="JR11" t="inlineStr">
-        <is>
-          <t>OFICIAL</t>
-        </is>
-      </c>
-      <c r="JS11" t="inlineStr">
-        <is>
-          <t>FRANCISCO JAVIER LOPEZ GUERRERO</t>
         </is>
       </c>
       <c r="JT11" t="inlineStr"/>

</xml_diff>